<commit_message>
Updated BEA and FRB pensions data
</commit_message>
<xml_diff>
--- a/data-raw/StatesBEAFRB/PensionEstimatesByState.xlsx
+++ b/data-raw/StatesBEAFRB/PensionEstimatesByState.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="115">
   <si>
     <t>Source:  U.S. Bureau of Economic Analysis</t>
   </si>
@@ -409,6 +409,9 @@
   </si>
   <si>
     <t>Last updated: September 26, 2017--new estimates for 2015; revised estimates for 2014.</t>
+  </si>
+  <si>
+    <t>Last updated: January 26, 2018--revised estimates for 2014 and 2015.</t>
   </si>
 </sst>
 </file>
@@ -737,6 +740,34 @@
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -1317,20 +1348,6 @@
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -1340,20 +1357,6 @@
           <color indexed="64"/>
         </top>
         <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1957,32 +1960,32 @@
     <tableColumn id="13" name="Column13" headerRowDxfId="43" dataDxfId="42"/>
     <tableColumn id="14" name="Column14" headerRowDxfId="41" dataDxfId="40"/>
     <tableColumn id="16" name="Column16" headerRowDxfId="39" dataDxfId="38"/>
-    <tableColumn id="15" name="Column15" headerRowDxfId="37" dataDxfId="36"/>
-    <tableColumn id="17" name="Column17" headerRowDxfId="35" dataDxfId="34"/>
+    <tableColumn id="15" name="Column15" headerRowDxfId="37" dataDxfId="1"/>
+    <tableColumn id="17" name="Column17" headerRowDxfId="36" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table7" displayName="Table7" ref="B6:Q56" headerRowCount="0" totalsRowShown="0" headerRowDxfId="33" tableBorderDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table7" displayName="Table7" ref="B6:Q56" headerRowCount="0" totalsRowShown="0" headerRowDxfId="35" tableBorderDxfId="34">
   <tableColumns count="16">
-    <tableColumn id="1" name="Column1" headerRowDxfId="31" dataDxfId="30" headerRowCellStyle="Normal_spi1204" dataCellStyle="Normal_spi1204"/>
-    <tableColumn id="2" name="Column2" headerRowDxfId="29" dataDxfId="28"/>
-    <tableColumn id="3" name="Column3" headerRowDxfId="27" dataDxfId="26"/>
-    <tableColumn id="4" name="Column4" headerRowDxfId="25" dataDxfId="24"/>
-    <tableColumn id="5" name="Column5" headerRowDxfId="23" dataDxfId="22"/>
-    <tableColumn id="6" name="Column6" headerRowDxfId="21" dataDxfId="20"/>
-    <tableColumn id="7" name="Column7" headerRowDxfId="19" dataDxfId="18"/>
-    <tableColumn id="8" name="Column8" headerRowDxfId="17" dataDxfId="16"/>
-    <tableColumn id="9" name="Column9" headerRowDxfId="15" dataDxfId="14"/>
-    <tableColumn id="10" name="Column10" headerRowDxfId="13" dataDxfId="12"/>
-    <tableColumn id="11" name="Column11" headerRowDxfId="11" dataDxfId="10"/>
-    <tableColumn id="12" name="Column12" headerRowDxfId="9" dataDxfId="8"/>
-    <tableColumn id="13" name="Column13" headerRowDxfId="7" dataDxfId="6"/>
-    <tableColumn id="14" name="Column14" headerRowDxfId="5" dataDxfId="4"/>
-    <tableColumn id="16" name="Column16" headerRowDxfId="3" dataDxfId="2"/>
-    <tableColumn id="17" name="Column17" headerRowDxfId="1" dataDxfId="0"/>
+    <tableColumn id="1" name="Column1" headerRowDxfId="33" dataDxfId="32" headerRowCellStyle="Normal_spi1204" dataCellStyle="Normal_spi1204"/>
+    <tableColumn id="2" name="Column2" headerRowDxfId="31" dataDxfId="30"/>
+    <tableColumn id="3" name="Column3" headerRowDxfId="29" dataDxfId="28"/>
+    <tableColumn id="4" name="Column4" headerRowDxfId="27" dataDxfId="26"/>
+    <tableColumn id="5" name="Column5" headerRowDxfId="25" dataDxfId="24"/>
+    <tableColumn id="6" name="Column6" headerRowDxfId="23" dataDxfId="22"/>
+    <tableColumn id="7" name="Column7" headerRowDxfId="21" dataDxfId="20"/>
+    <tableColumn id="8" name="Column8" headerRowDxfId="19" dataDxfId="18"/>
+    <tableColumn id="9" name="Column9" headerRowDxfId="17" dataDxfId="16"/>
+    <tableColumn id="10" name="Column10" headerRowDxfId="15" dataDxfId="14"/>
+    <tableColumn id="11" name="Column11" headerRowDxfId="13" dataDxfId="12"/>
+    <tableColumn id="12" name="Column12" headerRowDxfId="11" dataDxfId="10"/>
+    <tableColumn id="13" name="Column13" headerRowDxfId="9" dataDxfId="8"/>
+    <tableColumn id="14" name="Column14" headerRowDxfId="7" dataDxfId="6"/>
+    <tableColumn id="16" name="Column16" headerRowDxfId="5" dataDxfId="4"/>
+    <tableColumn id="17" name="Column17" headerRowDxfId="3" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2281,7 +2284,7 @@
   <dimension ref="A1:R58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2462,10 +2465,10 @@
         <v>4986903000</v>
       </c>
       <c r="Q5" s="9">
-        <v>5267288000</v>
+        <v>5236681000</v>
       </c>
       <c r="R5" s="9">
-        <v>5520855000</v>
+        <v>5488753000</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -2518,10 +2521,10 @@
         <v>51366180</v>
       </c>
       <c r="Q6" s="7">
-        <v>53920841</v>
+        <v>53607519</v>
       </c>
       <c r="R6" s="7">
-        <v>56071216</v>
+        <v>55745179</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -2574,10 +2577,10 @@
         <v>23279256</v>
       </c>
       <c r="Q7" s="9">
-        <v>25325346</v>
+        <v>25178187</v>
       </c>
       <c r="R7" s="9">
-        <v>26742559</v>
+        <v>26587060</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -2630,10 +2633,10 @@
         <v>70125296</v>
       </c>
       <c r="Q8" s="9">
-        <v>74856732</v>
+        <v>74421757</v>
       </c>
       <c r="R8" s="9">
-        <v>78267670</v>
+        <v>77812569</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -2686,10 +2689,10 @@
         <v>30273348</v>
       </c>
       <c r="Q9" s="9">
-        <v>31981984</v>
+        <v>31796144</v>
       </c>
       <c r="R9" s="9">
-        <v>33573961</v>
+        <v>33378739</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
@@ -2742,10 +2745,10 @@
         <v>955896156</v>
       </c>
       <c r="Q10" s="9">
-        <v>1014809436</v>
+        <v>1008912611</v>
       </c>
       <c r="R10" s="9">
-        <v>1062481735</v>
+        <v>1056303744</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
@@ -2798,10 +2801,10 @@
         <v>81786618</v>
       </c>
       <c r="Q11" s="9">
-        <v>85488334</v>
+        <v>84991581</v>
       </c>
       <c r="R11" s="9">
-        <v>88748268</v>
+        <v>88232226</v>
       </c>
     </row>
     <row r="12" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2854,10 +2857,10 @@
         <v>78657827</v>
       </c>
       <c r="Q12" s="9">
-        <v>82319326</v>
+        <v>81840987</v>
       </c>
       <c r="R12" s="9">
-        <v>87239785</v>
+        <v>86732513</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
@@ -2910,10 +2913,10 @@
         <v>10554688</v>
       </c>
       <c r="Q13" s="9">
-        <v>11062499</v>
+        <v>10998218</v>
       </c>
       <c r="R13" s="9">
-        <v>11976867</v>
+        <v>11907225</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
@@ -2966,10 +2969,10 @@
         <v>6597315</v>
       </c>
       <c r="Q14" s="9">
-        <v>7146953</v>
+        <v>7105423</v>
       </c>
       <c r="R14" s="9">
-        <v>7784270</v>
+        <v>7739007</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
@@ -3022,10 +3025,10 @@
         <v>208313114</v>
       </c>
       <c r="Q15" s="9">
-        <v>217859870</v>
+        <v>216593937</v>
       </c>
       <c r="R15" s="9">
-        <v>226735135</v>
+        <v>225416743</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
@@ -3078,10 +3081,10 @@
         <v>132036755</v>
       </c>
       <c r="Q16" s="9">
-        <v>138337590</v>
+        <v>137533742</v>
       </c>
       <c r="R16" s="9">
-        <v>144653520</v>
+        <v>143812406</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
@@ -3134,10 +3137,10 @@
         <v>23053314</v>
       </c>
       <c r="Q17" s="9">
-        <v>24262225</v>
+        <v>24121242</v>
       </c>
       <c r="R17" s="9">
-        <v>25507596</v>
+        <v>25359278</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
@@ -3190,10 +3193,10 @@
         <v>15201405</v>
       </c>
       <c r="Q18" s="9">
-        <v>16212918</v>
+        <v>16118708</v>
       </c>
       <c r="R18" s="9">
-        <v>17084788</v>
+        <v>16985446</v>
       </c>
     </row>
     <row r="19" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3246,10 +3249,10 @@
         <v>325768123</v>
       </c>
       <c r="Q19" s="9">
-        <v>345608813</v>
+        <v>343600558</v>
       </c>
       <c r="R19" s="9">
-        <v>364827932</v>
+        <v>362706575</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
@@ -3302,10 +3305,10 @@
         <v>38375603</v>
       </c>
       <c r="Q20" s="9">
-        <v>40748570</v>
+        <v>40511789</v>
       </c>
       <c r="R20" s="9">
-        <v>43867619</v>
+        <v>43612543</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
@@ -3358,10 +3361,10 @@
         <v>33320291</v>
       </c>
       <c r="Q21" s="9">
-        <v>35297363</v>
+        <v>35092258</v>
       </c>
       <c r="R21" s="9">
-        <v>37078008</v>
+        <v>36862411</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
@@ -3414,10 +3417,10 @@
         <v>26052463</v>
       </c>
       <c r="Q22" s="9">
-        <v>27261333</v>
+        <v>27102924</v>
       </c>
       <c r="R22" s="9">
-        <v>28341680</v>
+        <v>28176882</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
@@ -3470,10 +3473,10 @@
         <v>62241185</v>
       </c>
       <c r="Q23" s="9">
-        <v>65604558</v>
+        <v>65223345</v>
       </c>
       <c r="R23" s="9">
-        <v>68601793</v>
+        <v>68202895</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
@@ -3526,10 +3529,10 @@
         <v>73590977</v>
       </c>
       <c r="Q24" s="9">
-        <v>77083608</v>
+        <v>76635693</v>
       </c>
       <c r="R24" s="9">
-        <v>79764382</v>
+        <v>79300577</v>
       </c>
     </row>
     <row r="25" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3582,10 +3585,10 @@
         <v>15354639</v>
       </c>
       <c r="Q25" s="9">
-        <v>16004762</v>
+        <v>15911762</v>
       </c>
       <c r="R25" s="9">
-        <v>16445350</v>
+        <v>16349726</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
@@ -3638,10 +3641,10 @@
         <v>88363854</v>
       </c>
       <c r="Q26" s="9">
-        <v>93319105</v>
+        <v>92776849</v>
       </c>
       <c r="R26" s="9">
-        <v>98644287</v>
+        <v>98070702</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
@@ -3694,10 +3697,10 @@
         <v>135150166</v>
       </c>
       <c r="Q27" s="9">
-        <v>146109250</v>
+        <v>145260243</v>
       </c>
       <c r="R27" s="9">
-        <v>155647975</v>
+        <v>154742932</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
@@ -3750,10 +3753,10 @@
         <v>126174820</v>
       </c>
       <c r="Q28" s="9">
-        <v>130035570</v>
+        <v>129279963</v>
       </c>
       <c r="R28" s="9">
-        <v>131704181</v>
+        <v>130938364</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
@@ -3806,10 +3809,10 @@
         <v>78137620</v>
       </c>
       <c r="Q29" s="9">
-        <v>83670556</v>
+        <v>83184366</v>
       </c>
       <c r="R29" s="9">
-        <v>88699359</v>
+        <v>88183601</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
@@ -3862,10 +3865,10 @@
         <v>41314757</v>
       </c>
       <c r="Q30" s="9">
-        <v>44111997</v>
+        <v>43855673</v>
       </c>
       <c r="R30" s="9">
-        <v>46971389</v>
+        <v>46698266</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
@@ -3918,10 +3921,10 @@
         <v>96365014</v>
       </c>
       <c r="Q31" s="9">
-        <v>102107766</v>
+        <v>101514442</v>
       </c>
       <c r="R31" s="9">
-        <v>106475476</v>
+        <v>105856355</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
@@ -3974,10 +3977,10 @@
         <v>13235710</v>
       </c>
       <c r="Q32" s="9">
-        <v>14267650</v>
+        <v>14184744</v>
       </c>
       <c r="R32" s="9">
-        <v>14884995</v>
+        <v>14798444</v>
       </c>
     </row>
     <row r="33" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -4030,10 +4033,10 @@
         <v>18470570</v>
       </c>
       <c r="Q33" s="9">
-        <v>19446823</v>
+        <v>19333822</v>
       </c>
       <c r="R33" s="9">
-        <v>20349288</v>
+        <v>20230963</v>
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
@@ -4086,10 +4089,10 @@
         <v>47229012</v>
       </c>
       <c r="Q34" s="9">
-        <v>50104421</v>
+        <v>49813276</v>
       </c>
       <c r="R34" s="9">
-        <v>52990320</v>
+        <v>52682198</v>
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
@@ -4142,10 +4145,10 @@
         <v>11897486</v>
       </c>
       <c r="Q35" s="9">
-        <v>12498603</v>
+        <v>12425976</v>
       </c>
       <c r="R35" s="9">
-        <v>13296852</v>
+        <v>13219536</v>
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
@@ -4198,10 +4201,10 @@
         <v>167202664</v>
       </c>
       <c r="Q36" s="9">
-        <v>175361895</v>
+        <v>174342907</v>
       </c>
       <c r="R36" s="9">
-        <v>181592882</v>
+        <v>180536978</v>
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
@@ -4254,10 +4257,10 @@
         <v>38503846</v>
       </c>
       <c r="Q37" s="9">
-        <v>40862096</v>
+        <v>40624655</v>
       </c>
       <c r="R37" s="9">
-        <v>43370209</v>
+        <v>43118025</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
@@ -4310,10 +4313,10 @@
         <v>497782462</v>
       </c>
       <c r="Q38" s="9">
-        <v>523867224</v>
+        <v>520823150</v>
       </c>
       <c r="R38" s="9">
-        <v>548616937</v>
+        <v>545426907</v>
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
@@ -4366,10 +4369,10 @@
         <v>96235908</v>
       </c>
       <c r="Q39" s="9">
-        <v>100713335</v>
+        <v>100128113</v>
       </c>
       <c r="R39" s="9">
-        <v>106155308</v>
+        <v>105538049</v>
       </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
@@ -4422,10 +4425,10 @@
         <v>6561766</v>
       </c>
       <c r="Q40" s="9">
-        <v>7071782</v>
+        <v>7030690</v>
       </c>
       <c r="R40" s="9">
-        <v>7667090</v>
+        <v>7622508</v>
       </c>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
@@ -4478,10 +4481,10 @@
         <v>243953777</v>
       </c>
       <c r="Q41" s="9">
-        <v>254291639</v>
+        <v>252814009</v>
       </c>
       <c r="R41" s="9">
-        <v>263927487</v>
+        <v>262392833</v>
       </c>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
@@ -4534,10 +4537,10 @@
         <v>39401583</v>
       </c>
       <c r="Q42" s="9">
-        <v>41407231</v>
+        <v>41166623</v>
       </c>
       <c r="R42" s="9">
-        <v>43319250</v>
+        <v>43067363</v>
       </c>
     </row>
     <row r="43" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4590,10 +4593,10 @@
         <v>73070126</v>
       </c>
       <c r="Q43" s="9">
-        <v>80278506</v>
+        <v>79812026</v>
       </c>
       <c r="R43" s="9">
-        <v>89066496</v>
+        <v>88548603</v>
       </c>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
@@ -4646,10 +4649,10 @@
         <v>186825237</v>
       </c>
       <c r="Q44" s="9">
-        <v>193897368</v>
+        <v>192770675</v>
       </c>
       <c r="R44" s="9">
-        <v>201584506</v>
+        <v>200412357</v>
       </c>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
@@ -4702,10 +4705,10 @@
         <v>16428740</v>
       </c>
       <c r="Q45" s="9">
-        <v>16956502</v>
+        <v>16857972</v>
       </c>
       <c r="R45" s="9">
-        <v>17706833</v>
+        <v>17603873</v>
       </c>
     </row>
     <row r="46" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -4758,10 +4761,10 @@
         <v>51671662</v>
       </c>
       <c r="Q46" s="9">
-        <v>53975765</v>
+        <v>53662125</v>
       </c>
       <c r="R46" s="9">
-        <v>55833267</v>
+        <v>55508614</v>
       </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
@@ -4814,10 +4817,10 @@
         <v>14510596</v>
       </c>
       <c r="Q47" s="9">
-        <v>15906963</v>
+        <v>15814532</v>
       </c>
       <c r="R47" s="9">
-        <v>16812714</v>
+        <v>16714953</v>
       </c>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.25">
@@ -4870,10 +4873,10 @@
         <v>52297384</v>
       </c>
       <c r="Q48" s="9">
-        <v>54856543</v>
+        <v>54537785</v>
       </c>
       <c r="R48" s="9">
-        <v>56985183</v>
+        <v>56653832</v>
       </c>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.25">
@@ -4926,10 +4929,10 @@
         <v>252705615</v>
       </c>
       <c r="Q49" s="9">
-        <v>270725679</v>
+        <v>269152554</v>
       </c>
       <c r="R49" s="9">
-        <v>289696429</v>
+        <v>288011937</v>
       </c>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.25">
@@ -4982,10 +4985,10 @@
         <v>29157155</v>
       </c>
       <c r="Q50" s="9">
-        <v>30518784</v>
+        <v>30341447</v>
       </c>
       <c r="R50" s="9">
-        <v>31843453</v>
+        <v>31658293</v>
       </c>
     </row>
     <row r="51" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -5038,10 +5041,10 @@
         <v>6499316</v>
       </c>
       <c r="Q51" s="9">
-        <v>6959786</v>
+        <v>6919344</v>
       </c>
       <c r="R51" s="9">
-        <v>7350716</v>
+        <v>7307974</v>
       </c>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.25">
@@ -5094,10 +5097,10 @@
         <v>100867276</v>
       </c>
       <c r="Q52" s="9">
-        <v>105935100</v>
+        <v>105319536</v>
       </c>
       <c r="R52" s="9">
-        <v>110510162</v>
+        <v>109867581</v>
       </c>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.25">
@@ -5150,10 +5153,10 @@
         <v>89257635</v>
       </c>
       <c r="Q53" s="9">
-        <v>95951796</v>
+        <v>95394242</v>
       </c>
       <c r="R53" s="9">
-        <v>98306437</v>
+        <v>97734817</v>
       </c>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.25">
@@ -5206,10 +5209,10 @@
         <v>17709371</v>
       </c>
       <c r="Q54" s="9">
-        <v>18529382</v>
+        <v>18421712</v>
       </c>
       <c r="R54" s="9">
-        <v>19319727</v>
+        <v>19207389</v>
       </c>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.25">
@@ -5262,10 +5265,10 @@
         <v>78746905</v>
       </c>
       <c r="Q55" s="9">
-        <v>82294218</v>
+        <v>81816026</v>
       </c>
       <c r="R55" s="9">
-        <v>85118681</v>
+        <v>84623743</v>
       </c>
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.25">
@@ -5318,10 +5321,10 @@
         <v>9330414</v>
       </c>
       <c r="Q56" s="9">
-        <v>10061604</v>
+        <v>10003138</v>
       </c>
       <c r="R56" s="9">
-        <v>10612977</v>
+        <v>10551266</v>
       </c>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.25">
@@ -5348,7 +5351,7 @@
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58" s="25" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B58" s="24"/>
       <c r="C58" s="24"/>

</xml_diff>